<commit_message>
models from server db
</commit_message>
<xml_diff>
--- a/notebooks/dcat/source/DCAT_tw.xlsx
+++ b/notebooks/dcat/source/DCAT_tw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tw/Projects/ArchesProjects/Oslo/arches_datahub/notebooks/dcat/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4627556B-8E6B-C54E-8973-323D8DC0C98B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7652570F-D11E-824C-A9E8-F1A863BE25D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="960" windowWidth="46720" windowHeight="29240" firstSheet="1" activeTab="1" xr2:uid="{51F074EA-7002-4144-BC8A-DF1B160D803A}"/>
+    <workbookView xWindow="0" yWindow="960" windowWidth="46720" windowHeight="29240" firstSheet="1" activeTab="2" xr2:uid="{51F074EA-7002-4144-BC8A-DF1B160D803A}"/>
   </bookViews>
   <sheets>
     <sheet name="entiteiten" sheetId="4" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1004" uniqueCount="251">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="993" uniqueCount="246">
   <si>
     <t>Entiteit</t>
   </si>
@@ -550,9 +550,6 @@
     <t>Een e-mail adres in de vorm van een mailto URI volgens de standaard https://tools.ietf.org/html/rfc6068 .</t>
   </si>
   <si>
-    <t>https://data.vlaanderen.be/id/conceptscheme/dataserviceprotocol</t>
-  </si>
-  <si>
     <t>Dataservice.contactinformatie</t>
   </si>
   <si>
@@ -595,12 +592,6 @@
     <t>landingspagina</t>
   </si>
   <si>
-    <t>https://data.vlaanderen.be/id/conceptscheme/levensfase</t>
-  </si>
-  <si>
-    <t>https://data.vlaanderen.be/id/conceptscheme/ontwikkelingstoestand</t>
-  </si>
-  <si>
     <t>Dataservice.statuut</t>
   </si>
   <si>
@@ -739,9 +730,6 @@
     <t>Vlaamse open data</t>
   </si>
   <si>
-    <t>http://publications.europa.eu/resource/authority/file-type</t>
-  </si>
-  <si>
     <t>Distributie.identificator</t>
   </si>
   <si>
@@ -776,9 +764,6 @@
   </si>
   <si>
     <t>Een dataservice die deze distributie aanbiedt.</t>
-  </si>
-  <si>
-    <t>https://www.iana.org/assignments/media-types/media-types.xhtml</t>
   </si>
   <si>
     <t xml:space="preserve">
@@ -864,7 +849,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -874,12 +859,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -946,29 +925,29 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1956,8 +1935,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D684835F-B97C-43FD-8866-1762957E3A54}">
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView topLeftCell="J1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3:K46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="178.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2009,19 +1988,19 @@
       </c>
     </row>
     <row r="2" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="9"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="9"/>
-      <c r="G2" s="9"/>
-      <c r="H2" s="9"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
+      <c r="H2" s="5"/>
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
     </row>
     <row r="3" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -2030,7 +2009,7 @@
       <c r="B3" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="10" t="s">
         <v>108</v>
       </c>
       <c r="D3" s="2" t="s">
@@ -2056,377 +2035,377 @@
       </c>
     </row>
     <row r="4" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
-      <c r="G4" s="9"/>
-      <c r="H4" s="9"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-    </row>
-    <row r="5" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A5" s="6" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="5"/>
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+    </row>
+    <row r="5" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="D5" s="6" t="s">
+      <c r="D5" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G5" s="6" t="s">
+      <c r="G5" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I5" s="7" t="s">
+      <c r="I5" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="J5" s="7" t="s">
+      <c r="J5" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="6" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A6" s="6" t="s">
+    <row r="6" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="C6" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="D6" s="6" t="s">
+      <c r="D6" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="6">
+      <c r="F6" s="2">
         <v>1</v>
       </c>
-      <c r="G6" s="6" t="s">
+      <c r="G6" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I6" s="7" t="s">
+      <c r="I6" s="3" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="7" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A7" s="6" t="s">
+    <row r="7" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="2" t="s">
         <v>122</v>
       </c>
-      <c r="D7" s="6" t="s">
+      <c r="D7" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="F7" s="6" t="s">
+      <c r="F7" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G7" s="6" t="s">
+      <c r="G7" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I7" s="7" t="s">
+      <c r="I7" s="3" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="8" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A8" s="6" t="s">
+    <row r="8" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="F8" s="6" t="s">
+      <c r="F8" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G8" s="6" t="s">
+      <c r="G8" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I8" s="7" t="s">
+      <c r="I8" s="3" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="9" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A9" s="6" t="s">
+    <row r="9" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="E9" s="6" t="s">
+      <c r="E9" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="2">
         <v>1</v>
       </c>
-      <c r="G9" s="6" t="s">
+      <c r="G9" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I9" s="7" t="s">
+      <c r="I9" s="3" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="10" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A10" s="6" t="s">
+    <row r="10" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="E10" s="6" t="s">
+      <c r="E10" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="F10" s="6">
+      <c r="F10" s="2">
         <v>1</v>
       </c>
-      <c r="G10" s="6" t="s">
+      <c r="G10" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="7" t="s">
+      <c r="I10" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="J10" s="7" t="s">
+      <c r="J10" s="3" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="11" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A11" s="6" t="s">
+    <row r="11" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="10" t="s">
         <v>138</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E11" s="6" t="s">
+      <c r="E11" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="G11" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="7" t="s">
+      <c r="I11" s="3" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="12" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A12" s="6" t="s">
+    <row r="12" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="E12" s="6" t="s">
+      <c r="E12" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="F12" s="6" t="s">
+      <c r="F12" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I12" s="7" t="s">
+      <c r="I12" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="J12" s="7" t="s">
+      <c r="J12" s="3" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A13" s="6" t="s">
+    <row r="13" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D13" s="6" t="s">
+      <c r="D13" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E13" s="6" t="s">
+      <c r="E13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F13" s="6">
+      <c r="F13" s="2">
         <v>1</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H13" s="6" t="s">
+      <c r="H13" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="7" t="s">
+      <c r="I13" s="3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A14" s="11" t="s">
-        <v>247</v>
-      </c>
-      <c r="B14" s="12"/>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="13"/>
-      <c r="J14" s="13"/>
-      <c r="K14" s="13"/>
-    </row>
-    <row r="15" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A15" s="6" t="s">
+    <row r="14" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A14" s="7" t="s">
+        <v>242</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+      <c r="G14" s="8"/>
+      <c r="H14" s="8"/>
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+    </row>
+    <row r="15" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="D15" s="6" t="s">
+      <c r="D15" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E15" s="6" t="s">
+      <c r="E15" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F15" s="6" t="s">
+      <c r="F15" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="6" t="s">
+      <c r="G15" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="H15" s="6" t="s">
+      <c r="H15" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="3" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="16" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A16" s="6" t="s">
+    <row r="16" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="2" t="s">
         <v>153</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="D16" s="6" t="s">
+      <c r="D16" s="2" t="s">
         <v>155</v>
       </c>
-      <c r="E16" s="6" t="s">
+      <c r="E16" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="F16" s="6">
+      <c r="F16" s="2">
         <v>1</v>
       </c>
-      <c r="G16" s="6" t="s">
+      <c r="G16" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H16" s="6" t="s">
+      <c r="H16" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I16" s="7" t="s">
+      <c r="I16" s="3" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A17" s="11" t="s">
-        <v>248</v>
-      </c>
-      <c r="B17" s="12"/>
-      <c r="C17" s="12"/>
-      <c r="D17" s="12"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="12"/>
-      <c r="G17" s="12"/>
-      <c r="H17" s="12"/>
-      <c r="I17" s="13"/>
-      <c r="J17" s="13"/>
-      <c r="K17" s="13"/>
+      <c r="A17" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="9"/>
     </row>
     <row r="18" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -2435,7 +2414,7 @@
       <c r="B18" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="10" t="s">
         <v>160</v>
       </c>
       <c r="D18" s="2" t="s">
@@ -2493,105 +2472,105 @@
       </c>
     </row>
     <row r="20" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A20" s="11" t="s">
+      <c r="A20" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="12"/>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="12"/>
-      <c r="F20" s="12"/>
-      <c r="G20" s="12"/>
-      <c r="H20" s="12"/>
-      <c r="I20" s="13"/>
-      <c r="J20" s="13"/>
-      <c r="K20" s="13"/>
-    </row>
-    <row r="21" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A21" s="6" t="s">
+      <c r="B20" s="8"/>
+      <c r="C20" s="8"/>
+      <c r="D20" s="8"/>
+      <c r="E20" s="8"/>
+      <c r="F20" s="8"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="8"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="9"/>
+      <c r="K20" s="9"/>
+    </row>
+    <row r="21" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D21" s="6" t="s">
+      <c r="D21" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E21" s="6" t="s">
+      <c r="E21" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F21" s="6">
+      <c r="F21" s="2">
         <v>1</v>
       </c>
-      <c r="G21" s="6" t="s">
+      <c r="G21" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H21" s="6" t="s">
+      <c r="H21" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I21" s="7" t="s">
+      <c r="I21" s="3" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="22" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="6" t="s">
+    <row r="22" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F22" s="2">
+        <v>1</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>170</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>118</v>
-      </c>
-      <c r="D22" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="E22" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F22" s="6">
+    </row>
+    <row r="23" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F23" s="2">
         <v>1</v>
       </c>
-      <c r="G22" s="6" t="s">
+      <c r="G23" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="H22" s="6" t="s">
+      <c r="H23" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="I22" s="7" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="23" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A23" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B23" s="6" t="s">
-        <v>172</v>
-      </c>
-      <c r="C23" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="I23" s="3" t="s">
         <v>174</v>
-      </c>
-      <c r="E23" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="F23" s="6">
-        <v>1</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>111</v>
-      </c>
-      <c r="H23" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="I23" s="7" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="24" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2599,13 +2578,13 @@
         <v>24</v>
       </c>
       <c r="B24" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C24" s="2" t="s">
+      <c r="D24" s="2" t="s">
         <v>177</v>
-      </c>
-      <c r="D24" s="2" t="s">
-        <v>178</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>71</v>
@@ -2620,7 +2599,7 @@
         <v>23</v>
       </c>
       <c r="I24" s="3" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="25" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2628,7 +2607,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C25" s="2" t="s">
         <v>131</v>
@@ -2649,7 +2628,7 @@
         <v>23</v>
       </c>
       <c r="I25" s="3" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="26" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2657,13 +2636,13 @@
         <v>24</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>74</v>
@@ -2678,13 +2657,13 @@
         <v>23</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J26" s="3" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="K26" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="27" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2692,7 +2671,7 @@
         <v>24</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C27" s="2" t="s">
         <v>142</v>
@@ -2713,7 +2692,7 @@
         <v>23</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="J27" s="3" t="s">
         <v>152</v>
@@ -2724,13 +2703,13 @@
         <v>24</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>74</v>
@@ -2745,29 +2724,29 @@
         <v>23</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="J28" s="3" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="K28" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="16" x14ac:dyDescent="0.2">
-      <c r="A29" s="11" t="s">
+      <c r="A29" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B29" s="12"/>
-      <c r="C29" s="12"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="12"/>
-      <c r="F29" s="12"/>
-      <c r="G29" s="12"/>
-      <c r="H29" s="12"/>
-      <c r="I29" s="13"/>
-      <c r="J29" s="13"/>
-      <c r="K29" s="13"/>
+      <c r="B29" s="8"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="8"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
     </row>
     <row r="30" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
@@ -2776,7 +2755,7 @@
       <c r="B30" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C30" s="14" t="s">
+      <c r="C30" s="10" t="s">
         <v>145</v>
       </c>
       <c r="D30" s="2" t="s">
@@ -2803,7 +2782,7 @@
         <v>27</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C31" s="2" t="s">
         <v>115</v>
@@ -2824,7 +2803,7 @@
         <v>23</v>
       </c>
       <c r="I31" s="3" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="J31" s="3" t="s">
         <v>152</v>
@@ -2835,7 +2814,7 @@
         <v>27</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C32" s="2" t="s">
         <v>118</v>
@@ -2856,7 +2835,7 @@
         <v>23</v>
       </c>
       <c r="I32" s="3" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="33" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2864,13 +2843,13 @@
         <v>27</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>30</v>
@@ -2885,7 +2864,7 @@
         <v>23</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="34" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2893,7 +2872,7 @@
         <v>27</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="C34" s="2" t="s">
         <v>131</v>
@@ -2914,7 +2893,7 @@
         <v>23</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="35" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2922,13 +2901,13 @@
         <v>27</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>218</v>
-      </c>
-      <c r="C35" s="14" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>181</v>
+      </c>
+      <c r="D35" s="2" t="s">
         <v>182</v>
-      </c>
-      <c r="D35" s="2" t="s">
-        <v>183</v>
       </c>
       <c r="E35" s="2" t="s">
         <v>71</v>
@@ -2943,10 +2922,10 @@
         <v>23</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="J35" s="3" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
     </row>
     <row r="36" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2954,13 +2933,13 @@
         <v>27</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>74</v>
@@ -2975,13 +2954,13 @@
         <v>23</v>
       </c>
       <c r="I36" s="3" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="J36" s="3" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="K36" s="3" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="37" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -2989,13 +2968,13 @@
         <v>27</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>223</v>
-      </c>
-      <c r="C37" s="14" t="s">
-        <v>192</v>
+        <v>220</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>189</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="E37" s="2" t="s">
         <v>74</v>
@@ -3010,13 +2989,13 @@
         <v>23</v>
       </c>
       <c r="I37" s="3" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="J37" s="3" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="K37" s="3" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="38" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -3024,7 +3003,7 @@
         <v>27</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C38" s="2" t="s">
         <v>142</v>
@@ -3045,7 +3024,7 @@
         <v>23</v>
       </c>
       <c r="I38" s="3" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="J38" s="3" t="s">
         <v>152</v>
@@ -3056,13 +3035,13 @@
         <v>27</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E39" s="2" t="s">
         <v>74</v>
@@ -3077,13 +3056,13 @@
         <v>23</v>
       </c>
       <c r="I39" s="3" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="J39" s="3" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="K39" s="3" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
     <row r="40" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -3091,13 +3070,13 @@
         <v>27</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E40" s="2" t="s">
         <v>65</v>
@@ -3112,38 +3091,38 @@
         <v>23</v>
       </c>
       <c r="I40" s="3" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="J40" s="3" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="K40" s="3" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="41" spans="1:11" s="7" customFormat="1" ht="16" x14ac:dyDescent="0.2">
-      <c r="A41" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="B41" s="12" t="s">
-        <v>249</v>
-      </c>
-      <c r="C41" s="12"/>
-      <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="12"/>
-      <c r="G41" s="12"/>
-      <c r="H41" s="12"/>
-      <c r="I41" s="13"/>
-      <c r="J41" s="13"/>
-      <c r="K41" s="13"/>
+        <v>228</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" ht="16" x14ac:dyDescent="0.2">
+      <c r="A41" s="7" t="s">
+        <v>245</v>
+      </c>
+      <c r="B41" s="8" t="s">
+        <v>244</v>
+      </c>
+      <c r="C41" s="8"/>
+      <c r="D41" s="8"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="8"/>
+      <c r="G41" s="8"/>
+      <c r="H41" s="8"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
     </row>
     <row r="42" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>30</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>131</v>
@@ -3164,7 +3143,7 @@
         <v>23</v>
       </c>
       <c r="I42" s="3" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
     </row>
     <row r="43" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -3172,7 +3151,7 @@
         <v>30</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C43" s="2" t="s">
         <v>134</v>
@@ -3193,7 +3172,7 @@
         <v>23</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
     </row>
     <row r="44" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -3201,7 +3180,7 @@
         <v>30</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C44" s="2" t="s">
         <v>142</v>
@@ -3222,7 +3201,7 @@
         <v>23</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="J44" s="3" t="s">
         <v>152</v>
@@ -3233,10 +3212,10 @@
         <v>30</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="C45" s="14" t="s">
-        <v>240</v>
+        <v>235</v>
+      </c>
+      <c r="C45" s="10" t="s">
+        <v>236</v>
       </c>
       <c r="D45" s="2" t="s">
         <v>83</v>
@@ -3254,7 +3233,7 @@
         <v>23</v>
       </c>
       <c r="I45" s="3" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
     </row>
     <row r="46" spans="1:11" s="3" customFormat="1" ht="16" x14ac:dyDescent="0.2">
@@ -3262,10 +3241,10 @@
         <v>30</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="D46" s="2" t="s">
         <v>85</v>
@@ -3283,7 +3262,7 @@
         <v>23</v>
       </c>
       <c r="I46" s="3" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
@@ -3349,7 +3328,7 @@
     <row r="53" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A53" s="1"/>
       <c r="B53" s="1"/>
-      <c r="C53" s="1"/>
+      <c r="C53" s="11"/>
       <c r="D53" s="1"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
@@ -3358,1484 +3337,1480 @@
     </row>
     <row r="54" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C54" s="1"/>
       <c r="D54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H54" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="55" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>246</v>
-      </c>
+        <v>241</v>
+      </c>
+      <c r="C55" s="11"/>
       <c r="D55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H55" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="56" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H56" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H57" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="58" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H58" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="59" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H59" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="60" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H60" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="61" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H61" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H62" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="63" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H63" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="64" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H64" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="65" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H65" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H66" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H67" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H68" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="69" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H69" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H70" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H71" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H72" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H73" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H74" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H75" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H76" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H77" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H78" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H79" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H80" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H81" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H82" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H83" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="84" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H84" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="85" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H85" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="86" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H86" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H87" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H88" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H89" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="90" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H90" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="91" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H91" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="92" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H92" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H93" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="94" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H94" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="95" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H95" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="96" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H96" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="97" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H97" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="98" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H98" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="99" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H99" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="100" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H100" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="101" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H101" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="102" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H102" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="103" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H103" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="104" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H104" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="105" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H105" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="106" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H106" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="107" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H107" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="108" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H108" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="109" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H109" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
     <row r="110" spans="1:8" ht="32" x14ac:dyDescent="0.2">
       <c r="A110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="B110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="E110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="F110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="G110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="H110" s="1" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -4847,190 +4822,68 @@
     <hyperlink ref="C3" r:id="rId4" xr:uid="{81E66500-D18D-C643-B4A2-7DC6DF6D37F6}"/>
     <hyperlink ref="C18" r:id="rId5" xr:uid="{B5A30BB7-C00E-214A-8990-31D80A240BFA}"/>
     <hyperlink ref="C45" r:id="rId6" location="accessURL" xr:uid="{6A5821EF-BE85-734A-B738-EB86F0690206}"/>
+    <hyperlink ref="C11" r:id="rId7" location="record" xr:uid="{BE141BF8-DAB8-8E40-BC64-65946382D30D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD28AE82-F90F-5540-A27D-A74C55BD1DB0}">
-  <dimension ref="A1:A86"/>
+  <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="22.33203125" style="12" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
-        <v>203</v>
+      <c r="A1" s="12" t="s">
+        <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
-        <v>203</v>
+      <c r="A2" s="12" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>232</v>
+      <c r="A3" s="12" t="s">
+        <v>192</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>184</v>
+      <c r="A4" s="12" t="s">
+        <v>228</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
-        <v>195</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="5" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="4" t="s">
-        <v>231</v>
-      </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="3"/>
+      <c r="A6" s="13"/>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="3"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="3"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="4"/>
+      <c r="A16" s="14"/>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="4"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="3"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="3"/>
+      <c r="A19" s="14"/>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="4"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="3"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="3"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="4"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="3"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="3"/>
+      <c r="A22" s="14"/>
+    </row>
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A29" s="14"/>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="3"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="3"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="3"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="3"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="3"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="3"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="3"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="3"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="3"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="3"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="4"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="3"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="3"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="3"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="3"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="3"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="4"/>
+      <c r="A37" s="14"/>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A183">
-    <sortCondition ref="A1:A183"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A84">
+    <sortCondition ref="A1:A84"/>
   </sortState>
-  <hyperlinks>
-    <hyperlink ref="A11" r:id="rId1" xr:uid="{568C126E-4BA7-0D4B-B553-4857A1FF1AEB}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -5086,6 +4939,31 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="22b93d9f-f3ea-48c9-815f-d6424016a017">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <_dlc_DocId xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7">KC4XRV7TJSC2-1289807282-84</_dlc_DocId>
+    <_dlc_DocIdUrl xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7">
+      <Url>https://digipolis.sharepoint.com/teams/TVBenBDigitalewerkingintern/_layouts/15/DocIdRedir.aspx?ID=KC4XRV7TJSC2-1289807282-84</Url>
+      <Description>KC4XRV7TJSC2-1289807282-84</Description>
+    </_dlc_DocIdUrl>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A837DF111CA6F34685ECF19F6D1B905A" ma:contentTypeVersion="15" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="2cf5797db51caa311d5fcf99b3a57fdf">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="02131b35-df3a-4512-bab4-ab3ae049f2a7" xmlns:ns3="22b93d9f-f3ea-48c9-815f-d6424016a017" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="fa7e433c227d2d68eede10c3930b990f" ns2:_="" ns3:_="">
     <xsd:import namespace="02131b35-df3a-4512-bab4-ab3ae049f2a7"/>
@@ -5345,31 +5223,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="22b93d9f-f3ea-48c9-815f-d6424016a017">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <_dlc_DocId xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7">KC4XRV7TJSC2-1289807282-84</_dlc_DocId>
-    <_dlc_DocIdUrl xmlns="02131b35-df3a-4512-bab4-ab3ae049f2a7">
-      <Url>https://digipolis.sharepoint.com/teams/TVBenBDigitalewerkingintern/_layouts/15/DocIdRedir.aspx?ID=KC4XRV7TJSC2-1289807282-84</Url>
-      <Description>KC4XRV7TJSC2-1289807282-84</Description>
-    </_dlc_DocIdUrl>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item4.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2AF1EC21-D20F-4E16-BF1E-91258DFB0951}">
   <ds:schemaRefs>
@@ -5379,6 +5232,25 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6861A1EF-F5F0-4BF1-8BDE-BFA0A5220173}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D3C55B9-FB24-4E22-9941-92D738592EB3}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="02131b35-df3a-4512-bab4-ab3ae049f2a7"/>
+    <ds:schemaRef ds:uri="22b93d9f-f3ea-48c9-815f-d6424016a017"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{249F1D2F-18DC-4E8B-A45A-6458FECBB1A1}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -5395,23 +5267,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9D3C55B9-FB24-4E22-9941-92D738592EB3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="02131b35-df3a-4512-bab4-ab3ae049f2a7"/>
-    <ds:schemaRef ds:uri="22b93d9f-f3ea-48c9-815f-d6424016a017"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps4.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6861A1EF-F5F0-4BF1-8BDE-BFA0A5220173}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
DCAT models and rdfs
</commit_message>
<xml_diff>
--- a/notebooks/dcat/source/DCAT_tw.xlsx
+++ b/notebooks/dcat/source/DCAT_tw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tw/Projects/ArchesProjects/Oslo/arches_datahub/notebooks/dcat/source/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7652570F-D11E-824C-A9E8-F1A863BE25D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4DA9E401-1196-CF4B-8538-0F2C0370E5AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="960" windowWidth="46720" windowHeight="29240" firstSheet="1" activeTab="2" xr2:uid="{51F074EA-7002-4144-BC8A-DF1B160D803A}"/>
+    <workbookView xWindow="0" yWindow="960" windowWidth="46720" windowHeight="29240" firstSheet="1" activeTab="1" xr2:uid="{51F074EA-7002-4144-BC8A-DF1B160D803A}"/>
   </bookViews>
   <sheets>
     <sheet name="entiteiten" sheetId="4" r:id="rId1"/>
@@ -916,7 +916,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -948,6 +948,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1935,8 +1936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D684835F-B97C-43FD-8866-1762957E3A54}">
   <dimension ref="A1:K110"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <selection activeCell="K3" sqref="K3:K46"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="178.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -4833,22 +4834,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD28AE82-F90F-5540-A27D-A74C55BD1DB0}">
   <dimension ref="A1:A37"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView zoomScale="186" zoomScaleNormal="186" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.33203125" style="12" customWidth="1"/>
+    <col min="1" max="1" width="49.33203125" style="12" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="12" t="s">
+      <c r="A1" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="15" t="s">
         <v>188</v>
       </c>
     </row>
@@ -4884,6 +4885,9 @@
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A84">
     <sortCondition ref="A1:A84"/>
   </sortState>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{BF689387-068D-5946-A966-F9E3642201BC}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>